<commit_message>
Revert "Merge branch 'master' of https://github.com/MrGonzalezCruz/SIGECU_1.0.0"
This reverts commit f132e10f7f8c05353a651fa297a3c88f28adf669, reversing
changes made to f88d44f34deba77eb7a8cff651ff7f811f570325.
</commit_message>
<xml_diff>
--- a/Documentation/FASOFT Acividades Release 2.xlsx
+++ b/Documentation/FASOFT Acividades Release 2.xlsx
@@ -297,7 +297,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -335,6 +335,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -465,17 +469,17 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.05"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.0202429149798"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="73.3765182186235"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.0283400809717"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -486,7 +490,6 @@
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -499,7 +502,6 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -516,7 +518,6 @@
       <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
@@ -534,9 +535,6 @@
       </c>
       <c r="F4" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,11 +543,11 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="10" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="1" t="n">
@@ -562,11 +560,11 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="10" t="n">
         <v>5</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="1" t="n">
@@ -577,23 +575,23 @@
       <c r="A7" s="0"/>
       <c r="B7" s="0"/>
       <c r="C7" s="0"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="0"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="10" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="1" t="n">
@@ -601,18 +599,18 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="10" t="n">
         <v>5</v>
       </c>
       <c r="E9" s="8" t="n">
         <v>0.75</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="1" t="n">
@@ -620,77 +618,68 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="10" t="n">
         <v>3</v>
       </c>
       <c r="E10" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="0" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="4"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="10" t="n">
         <v>5</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="14" t="s">
         <v>13</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="0"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="D13" s="10" t="n">
         <v>5</v>
       </c>
       <c r="E13" s="8" t="n">
         <v>0.4</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="20" t="s">
         <v>21</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="4"/>
       <c r="C14" s="0"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="0"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
@@ -700,11 +689,10 @@
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="0"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
@@ -717,7 +705,7 @@
       <c r="E16" s="8" t="n">
         <v>0.4</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="18" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="1" t="n">
@@ -725,7 +713,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
@@ -738,15 +726,12 @@
       <c r="E17" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="0"/>
       <c r="C18" s="1" t="s">
         <v>26</v>
@@ -757,7 +742,7 @@
       <c r="E18" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="1" t="n">
@@ -765,7 +750,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
@@ -778,15 +763,12 @@
       <c r="E19" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="0" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20"/>
+      <c r="A20" s="21"/>
       <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
@@ -799,7 +781,7 @@
       <c r="E20" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="22" t="s">
         <v>31</v>
       </c>
       <c r="G20" s="1" t="n">

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/MrGonzalezCruz/SIGECU_1.0.0""
This reverts commit 15c78b458ba523d0f79404e1f44db7069f47fb06.
</commit_message>
<xml_diff>
--- a/Documentation/FASOFT Acividades Release 2.xlsx
+++ b/Documentation/FASOFT Acividades Release 2.xlsx
@@ -297,7 +297,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -335,10 +335,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -469,17 +465,17 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.05"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="73.3765182186235"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="74.0202429149798"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="38.3481781376518"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -490,6 +486,7 @@
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
       <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -502,6 +499,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -518,6 +516,7 @@
       <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="G3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
@@ -535,6 +534,9 @@
       </c>
       <c r="F4" s="6" t="s">
         <v>7</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,11 +545,11 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="D5" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="1" t="n">
@@ -560,11 +562,11 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E6" s="8"/>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="1" t="n">
@@ -575,23 +577,23 @@
       <c r="A7" s="0"/>
       <c r="B7" s="0"/>
       <c r="C7" s="0"/>
-      <c r="D7" s="10"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="12"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10" t="n">
+      <c r="D8" s="1" t="n">
         <v>2</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="1" t="n">
@@ -599,18 +601,18 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E9" s="8" t="n">
         <v>0.75</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="1" t="n">
@@ -618,68 +620,77 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="4"/>
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="10" t="n">
+      <c r="D10" s="1" t="n">
         <v>3</v>
       </c>
       <c r="E10" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="17" t="s">
         <v>17</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="4"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="D11" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E11" s="8"/>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>13</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="0"/>
       <c r="C12" s="0"/>
-      <c r="D12" s="10"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="12"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="10" t="n">
+      <c r="D13" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E13" s="8" t="n">
         <v>0.4</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="19" t="s">
         <v>21</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="4"/>
       <c r="C14" s="0"/>
-      <c r="D14" s="10"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="12"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0"/>
@@ -689,10 +700,11 @@
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="12"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
@@ -705,7 +717,7 @@
       <c r="E16" s="8" t="n">
         <v>0.4</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="17" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="1" t="n">
@@ -713,7 +725,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
@@ -726,12 +738,15 @@
       <c r="E17" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="19" t="s">
         <v>21</v>
       </c>
+      <c r="G17" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="0"/>
       <c r="C18" s="1" t="s">
         <v>26</v>
@@ -742,7 +757,7 @@
       <c r="E18" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="15" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="1" t="n">
@@ -750,7 +765,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
@@ -763,12 +778,15 @@
       <c r="E19" s="8" t="n">
         <v>0.2</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="17" t="s">
         <v>17</v>
       </c>
+      <c r="G19" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="25.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
@@ -781,7 +799,7 @@
       <c r="E20" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="21" t="s">
         <v>31</v>
       </c>
       <c r="G20" s="1" t="n">

</xml_diff>